<commit_message>
update to change to cli
</commit_message>
<xml_diff>
--- a/testData/testActors.xlsx
+++ b/testData/testActors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MengSpring\data-692\project3\ENSF692-Project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MengSpring\data-692\ENSF692-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4263CCD3-8799-4C52-A73D-A781009E0DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D684F1A9-99D7-4FD8-BF97-2A82AA9BC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15930" yWindow="5295" windowWidth="21600" windowHeight="15585" xr2:uid="{55CB430D-324D-4D6A-8886-7B6AAF73252F}"/>
+    <workbookView xWindow="3790" yWindow="3450" windowWidth="19200" windowHeight="11170" xr2:uid="{55CB430D-324D-4D6A-8886-7B6AAF73252F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,10 +65,10 @@
     <t xml:space="preserve">eliza gonzalez </t>
   </si>
   <si>
-    <t>RDJ</t>
-  </si>
-  <si>
     <t>movie</t>
+  </si>
+  <si>
+    <t>rdj</t>
   </si>
 </sst>
 </file>
@@ -443,28 +443,28 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -496,7 +496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>

</xml_diff>